<commit_message>
removing stretch and rerunning
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliobotero/Dropbox/SUAVE/SUAVE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE807FB0-4458-2B45-AA8F-B95880114890}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CFEE6D-2289-F84E-B399-4DC49CB1F8E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="500" windowWidth="28900" windowHeight="20500" activeTab="1" xr2:uid="{046A4ECD-B913-D647-AEA1-3714B5C9A77F}"/>
+    <workbookView xWindow="4700" yWindow="500" windowWidth="28900" windowHeight="20500" activeTab="1" xr2:uid="{046A4ECD-B913-D647-AEA1-3714B5C9A77F}"/>
   </bookViews>
   <sheets>
     <sheet name="B_T_W only" sheetId="1" r:id="rId1"/>
@@ -24011,8 +24011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB84D9B7-4798-7E4F-A973-934ACEE97A60}">
   <dimension ref="B1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>